<commit_message>
Major refactor; improving PCA
</commit_message>
<xml_diff>
--- a/metrics/metricsOCSVM.xlsx
+++ b/metrics/metricsOCSVM.xlsx
@@ -66,6 +66,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,7 +448,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.47640585899353</v>
+        <v>4.473053169250488</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +458,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003590774536132812</v>
+        <v>0.009083986282348633</v>
       </c>
     </row>
     <row r="4">
@@ -400,7 +468,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6</v>
+        <v>0.7700000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -410,7 +478,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8247619047619047</v>
+        <v>0.9700534759358289</v>
       </c>
     </row>
     <row r="6">
@@ -420,7 +488,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2609615334935028</v>
+        <v>0.5585714285714285</v>
       </c>
     </row>
     <row r="7">
@@ -430,7 +498,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6</v>
+        <v>0.7700000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -440,7 +508,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5441904468399852</v>
+        <v>0.7552539755429658</v>
       </c>
     </row>
     <row r="9">
@@ -450,7 +518,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5465318127461845</v>
+        <v>0.7558471381924038</v>
       </c>
     </row>
     <row r="10">
@@ -469,10 +537,8 @@
           <t>gamma</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>scale</t>
-        </is>
+      <c r="B11" t="n">
+        <v>0.001</v>
       </c>
     </row>
     <row r="12">
@@ -483,7 +549,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>rbf</t>
+          <t>sigmoid</t>
         </is>
       </c>
     </row>

</xml_diff>